<commit_message>
67763 Sprint1 Scrum Update
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt Template.xlsx
+++ b/SE202526/Management/Gantt Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF865BCE-518C-4401-9706-71E7BD3908A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="8_{AF865BCE-518C-4401-9706-71E7BD3908A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90FFE113-FE1D-40B6-B1EB-4360D892B95B}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="1460" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Project Planner</t>
   </si>
@@ -50,45 +50,6 @@
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
   </si>
   <si>
     <t>Activity 14</t>
@@ -268,17 +229,38 @@
     <t>M3</t>
   </si>
   <si>
-    <t>S2, S3</t>
-  </si>
-  <si>
-    <t>S5,S6</t>
+    <t>67763, 67775, 68547</t>
+  </si>
+  <si>
+    <t>T1: Play the first area of the game.</t>
+  </si>
+  <si>
+    <t>67286, 67763, 67804</t>
+  </si>
+  <si>
+    <t>T2: Read through the classes in the codebase.</t>
+  </si>
+  <si>
+    <t>67286, 67763, 67775, 67804, 68130, 68547</t>
+  </si>
+  <si>
+    <t>T3: Define roughly functionality 1.</t>
+  </si>
+  <si>
+    <t>T4: Define roughly functionality 2.</t>
+  </si>
+  <si>
+    <t>T5: Define roughly functionality 3.</t>
+  </si>
+  <si>
+    <t>T6: Trial modification of code.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -314,11 +296,13 @@
       <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -378,6 +362,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="9">
@@ -636,18 +626,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -671,12 +667,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="19" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1088,23 +1078,23 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BP30"/>
+  <dimension ref="B1:BP23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="3.21875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" customWidth="1"/>
-    <col min="2" max="2" width="23.4140625" customWidth="1"/>
-    <col min="3" max="3" width="15.58203125" style="2" customWidth="1"/>
-    <col min="4" max="7" width="11.58203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.58203125" style="4" customWidth="1"/>
-    <col min="9" max="28" width="3.25" style="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="39.44140625" customWidth="1"/>
+    <col min="3" max="3" width="49.88671875" style="2" customWidth="1"/>
+    <col min="4" max="7" width="11.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="4" customWidth="1"/>
+    <col min="9" max="28" width="3.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:68" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
+    <row r="1" spans="2:68" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1104,7 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
@@ -1123,79 +1113,79 @@
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I2" s="14">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K2" s="15"/>
-      <c r="L2" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="30"/>
+      <c r="L2" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="32"/>
       <c r="Q2" s="16"/>
-      <c r="R2" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="30"/>
+      <c r="R2" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="32"/>
       <c r="V2" s="17"/>
-      <c r="W2" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="32"/>
+      <c r="W2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="34"/>
       <c r="AA2" s="18"/>
-      <c r="AB2" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="32"/>
+      <c r="AB2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="34"/>
       <c r="AI2" s="19"/>
-      <c r="AJ2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
-      <c r="AQ2" s="22"/>
-    </row>
-    <row r="3" spans="2:68" s="11" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="AJ2" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="26"/>
+      <c r="AP2" s="26"/>
+      <c r="AQ2" s="26"/>
+    </row>
+    <row r="3" spans="2:68" s="11" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>34</v>
+      <c r="D3" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>21</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
@@ -1209,30 +1199,30 @@
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
       <c r="X3" s="10"/>
-      <c r="Z3" s="33" t="s">
-        <v>48</v>
+      <c r="Z3" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="AI3" s="10" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="AJ3" s="10"/>
       <c r="AK3" s="10"/>
       <c r="AL3" s="10"/>
       <c r="AM3" s="10"/>
-      <c r="AN3" s="33" t="s">
-        <v>49</v>
+      <c r="AN3" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="AO3" s="10"/>
       <c r="AP3" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="AQ3" s="10"/>
       <c r="AR3" s="10"/>
@@ -1241,7 +1231,7 @@
       <c r="AU3" s="10"/>
       <c r="AV3" s="10"/>
       <c r="AW3" s="10" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="AX3" s="10"/>
       <c r="AY3" s="10"/>
@@ -1250,7 +1240,7 @@
       <c r="BB3" s="10"/>
       <c r="BC3" s="10"/>
       <c r="BD3" s="10" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="BE3" s="10"/>
       <c r="BF3" s="10"/>
@@ -1261,18 +1251,18 @@
       <c r="BK3" s="10"/>
       <c r="BL3" s="10"/>
       <c r="BM3" s="10"/>
-      <c r="BN3" s="33" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BN3" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="3">
         <v>1</v>
       </c>
@@ -1454,539 +1444,402 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="34" t="s">
+    <row r="5" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7">
+        <v>4</v>
+      </c>
+      <c r="G5" s="7">
+        <v>9</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D6" s="7">
         <v>5</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <v>4</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1</v>
       </c>
       <c r="E6" s="7">
         <v>6</v>
       </c>
       <c r="F6" s="7">
+        <v>2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>67775</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="7">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="7">
+      <c r="F7" s="7">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7">
+        <v>4</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="8">
+        <v>9</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>7</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="7">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>8</v>
+      </c>
+      <c r="G9" s="7">
+        <v>4</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>67775</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="7">
+        <v>11</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="7">
-        <v>2</v>
-      </c>
-      <c r="E7" s="7">
-        <v>4</v>
-      </c>
-      <c r="F7" s="7">
-        <v>2</v>
-      </c>
-      <c r="G7" s="7">
-        <v>5</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="7">
-        <v>4</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="7">
-        <v>4</v>
-      </c>
-      <c r="G8" s="7">
-        <v>6</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="7">
-        <v>4</v>
-      </c>
-      <c r="E9" s="7">
-        <v>2</v>
-      </c>
-      <c r="F9" s="7">
-        <v>4</v>
-      </c>
-      <c r="G9" s="7">
-        <v>8</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="7">
-        <v>4</v>
-      </c>
-      <c r="E10" s="7">
-        <v>3</v>
-      </c>
-      <c r="F10" s="7">
-        <v>4</v>
-      </c>
-      <c r="G10" s="7">
-        <v>6</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="11" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="6" t="s">
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7">
-        <v>5</v>
-      </c>
-      <c r="E11" s="7">
-        <v>4</v>
-      </c>
-      <c r="F11" s="7">
-        <v>5</v>
-      </c>
-      <c r="G11" s="7">
-        <v>3</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="6" t="s">
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7">
-        <v>5</v>
-      </c>
-      <c r="E12" s="7">
-        <v>2</v>
-      </c>
-      <c r="F12" s="7">
-        <v>5</v>
-      </c>
-      <c r="G12" s="7">
-        <v>5</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C13" s="6" t="s">
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="7">
-        <v>5</v>
-      </c>
-      <c r="E13" s="7">
-        <v>2</v>
-      </c>
-      <c r="F13" s="7">
-        <v>5</v>
-      </c>
-      <c r="G13" s="7">
-        <v>6</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="14" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="6" t="s">
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="7">
-        <v>6</v>
-      </c>
-      <c r="E14" s="7">
-        <v>5</v>
-      </c>
-      <c r="F14" s="7">
-        <v>6</v>
-      </c>
-      <c r="G14" s="7">
-        <v>7</v>
-      </c>
-      <c r="H14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C15" s="6" t="s">
+      <c r="D20" s="7">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="8">
-        <v>6</v>
-      </c>
-      <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7">
-        <v>5</v>
-      </c>
-      <c r="G15" s="7">
-        <v>8</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C16" s="6" t="s">
+      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="7">
-        <v>9</v>
-      </c>
-      <c r="E16" s="7">
-        <v>3</v>
-      </c>
-      <c r="F16" s="7">
-        <v>9</v>
-      </c>
-      <c r="G16" s="7">
-        <v>3</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="6" t="s">
+      <c r="D22" s="7">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="7">
-        <v>9</v>
-      </c>
-      <c r="E17" s="7">
-        <v>6</v>
-      </c>
-      <c r="F17" s="7">
-        <v>9</v>
-      </c>
-      <c r="G17" s="7">
-        <v>7</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="7">
-        <v>9</v>
-      </c>
-      <c r="E18" s="7">
-        <v>3</v>
-      </c>
-      <c r="F18" s="7">
-        <v>9</v>
-      </c>
-      <c r="G18" s="7">
-        <v>1</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="7">
-        <v>9</v>
-      </c>
-      <c r="E19" s="7">
-        <v>4</v>
-      </c>
-      <c r="F19" s="7">
-        <v>8</v>
-      </c>
-      <c r="G19" s="7">
-        <v>5</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="7">
-        <v>10</v>
-      </c>
-      <c r="E20" s="7">
-        <v>5</v>
-      </c>
-      <c r="F20" s="7">
-        <v>10</v>
-      </c>
-      <c r="G20" s="7">
-        <v>3</v>
-      </c>
-      <c r="H20" s="4">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="7">
-        <v>11</v>
-      </c>
-      <c r="E21" s="7">
-        <v>2</v>
-      </c>
-      <c r="F21" s="7">
-        <v>11</v>
-      </c>
-      <c r="G21" s="7">
-        <v>5</v>
-      </c>
-      <c r="H21" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="7">
-        <v>12</v>
-      </c>
-      <c r="E22" s="7">
-        <v>6</v>
-      </c>
-      <c r="F22" s="7">
-        <v>12</v>
-      </c>
-      <c r="G22" s="7">
-        <v>7</v>
-      </c>
-      <c r="H22" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C23" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="D23" s="7">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E23" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="7">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G23" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H23" s="4">
         <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="7">
-        <v>14</v>
-      </c>
-      <c r="E24" s="7">
-        <v>5</v>
-      </c>
-      <c r="F24" s="7">
-        <v>14</v>
-      </c>
-      <c r="G24" s="7">
-        <v>6</v>
-      </c>
-      <c r="H24" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="7">
-        <v>14</v>
-      </c>
-      <c r="E25" s="7">
-        <v>8</v>
-      </c>
-      <c r="F25" s="7">
-        <v>14</v>
-      </c>
-      <c r="G25" s="7">
-        <v>2</v>
-      </c>
-      <c r="H25" s="4">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C26" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="7">
-        <v>14</v>
-      </c>
-      <c r="E26" s="7">
-        <v>7</v>
-      </c>
-      <c r="F26" s="7">
-        <v>14</v>
-      </c>
-      <c r="G26" s="7">
-        <v>3</v>
-      </c>
-      <c r="H26" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C27" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="7">
-        <v>15</v>
-      </c>
-      <c r="E27" s="7">
-        <v>4</v>
-      </c>
-      <c r="F27" s="7">
-        <v>15</v>
-      </c>
-      <c r="G27" s="7">
-        <v>8</v>
-      </c>
-      <c r="H27" s="4">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C28" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="7">
-        <v>15</v>
-      </c>
-      <c r="E28" s="7">
-        <v>5</v>
-      </c>
-      <c r="F28" s="7">
-        <v>15</v>
-      </c>
-      <c r="G28" s="7">
-        <v>3</v>
-      </c>
-      <c r="H28" s="4">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C29" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="7">
-        <v>15</v>
-      </c>
-      <c r="E29" s="7">
-        <v>8</v>
-      </c>
-      <c r="F29" s="7">
-        <v>15</v>
-      </c>
-      <c r="G29" s="7">
-        <v>5</v>
-      </c>
-      <c r="H29" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="7">
-        <v>16</v>
-      </c>
-      <c r="E30" s="7">
-        <v>28</v>
-      </c>
-      <c r="F30" s="7">
-        <v>16</v>
-      </c>
-      <c r="G30" s="7">
-        <v>30</v>
-      </c>
-      <c r="H30" s="4">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -2004,7 +1857,8 @@
     <mergeCell ref="W2:Z2"/>
     <mergeCell ref="AB2:AH2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C31:BP31">
+  <phoneticPr fontId="14" type="noConversion"/>
+  <conditionalFormatting sqref="C24:BP24">
     <cfRule type="expression" dxfId="9" priority="2">
       <formula>TRUE</formula>
     </cfRule>
@@ -2014,7 +1868,7 @@
       <formula>I$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BP30">
+  <conditionalFormatting sqref="I5:BP23">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>